<commit_message>
rearanged file structure in project, new script saving geojson data
</commit_message>
<xml_diff>
--- a/data/interim/covid_data/population_county.xlsx
+++ b/data/interim/covid_data/population_county.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B381"/>
+  <dimension ref="A1:C381"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>ludnosc</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -454,6 +459,11 @@
       <c r="B2" t="n">
         <v>89762</v>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -464,6 +474,11 @@
       <c r="B3" t="n">
         <v>99935</v>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -474,6 +489,11 @@
       <c r="B4" t="n">
         <v>88447</v>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -484,6 +504,11 @@
       <c r="B5" t="n">
         <v>34552</v>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -494,6 +519,11 @@
       <c r="B6" t="n">
         <v>49734</v>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -504,6 +534,11 @@
       <c r="B7" t="n">
         <v>63333</v>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -514,6 +549,11 @@
       <c r="B8" t="n">
         <v>42824</v>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -524,6 +564,11 @@
       <c r="B9" t="n">
         <v>156283</v>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -534,6 +579,11 @@
       <c r="B10" t="n">
         <v>55110</v>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -544,6 +594,11 @@
       <c r="B11" t="n">
         <v>53852</v>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -554,6 +609,11 @@
       <c r="B12" t="n">
         <v>105896</v>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -564,6 +624,11 @@
       <c r="B13" t="n">
         <v>45599</v>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -574,6 +639,11 @@
       <c r="B14" t="n">
         <v>36800</v>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -584,6 +654,11 @@
       <c r="B15" t="n">
         <v>107268</v>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -594,6 +669,11 @@
       <c r="B16" t="n">
         <v>76733</v>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -604,6 +684,11 @@
       <c r="B17" t="n">
         <v>62997</v>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -614,6 +699,11 @@
       <c r="B18" t="n">
         <v>43221</v>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -624,6 +714,11 @@
       <c r="B19" t="n">
         <v>55508</v>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -634,6 +729,11 @@
       <c r="B20" t="n">
         <v>156015</v>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -644,6 +744,11 @@
       <c r="B21" t="n">
         <v>85226</v>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -654,6 +759,11 @@
       <c r="B22" t="n">
         <v>55107</v>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -664,6 +774,11 @@
       <c r="B23" t="n">
         <v>46623</v>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -674,6 +789,11 @@
       <c r="B24" t="n">
         <v>156322</v>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -684,6 +804,11 @@
       <c r="B25" t="n">
         <v>64080</v>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -694,6 +819,11 @@
       <c r="B26" t="n">
         <v>88386</v>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -704,6 +834,11 @@
       <c r="B27" t="n">
         <v>43038</v>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -714,6 +849,11 @@
       <c r="B28" t="n">
         <v>78335</v>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -724,6 +864,11 @@
       <c r="B29" t="n">
         <v>98436</v>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -734,6 +879,11 @@
       <c r="B30" t="n">
         <v>641928</v>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -744,6 +894,11 @@
       <c r="B31" t="n">
         <v>109971</v>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -754,6 +909,11 @@
       <c r="B32" t="n">
         <v>54891</v>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -764,6 +924,11 @@
       <c r="B33" t="n">
         <v>79023</v>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -774,6 +939,11 @@
       <c r="B34" t="n">
         <v>120432</v>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -784,6 +954,11 @@
       <c r="B35" t="n">
         <v>51657</v>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -794,6 +969,11 @@
       <c r="B36" t="n">
         <v>44855</v>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -804,6 +984,11 @@
       <c r="B37" t="n">
         <v>40305</v>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -814,6 +999,11 @@
       <c r="B38" t="n">
         <v>158496</v>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -824,6 +1014,11 @@
       <c r="B39" t="n">
         <v>65450</v>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -834,6 +1029,11 @@
       <c r="B40" t="n">
         <v>45482</v>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -844,6 +1044,11 @@
       <c r="B41" t="n">
         <v>86119</v>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -854,6 +1059,11 @@
       <c r="B42" t="n">
         <v>40025</v>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -864,6 +1074,11 @@
       <c r="B43" t="n">
         <v>43390</v>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -874,6 +1089,11 @@
       <c r="B44" t="n">
         <v>40826</v>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -884,6 +1104,11 @@
       <c r="B45" t="n">
         <v>98703</v>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -894,6 +1119,11 @@
       <c r="B46" t="n">
         <v>109565</v>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -904,6 +1134,11 @@
       <c r="B47" t="n">
         <v>48322</v>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -914,6 +1149,11 @@
       <c r="B48" t="n">
         <v>34040</v>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -924,6 +1164,11 @@
       <c r="B49" t="n">
         <v>85646</v>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -934,6 +1179,11 @@
       <c r="B50" t="n">
         <v>69886</v>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -944,6 +1194,11 @@
       <c r="B51" t="n">
         <v>344091</v>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -954,6 +1209,11 @@
       <c r="B52" t="n">
         <v>93564</v>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -964,6 +1224,11 @@
       <c r="B53" t="n">
         <v>198613</v>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -974,6 +1239,11 @@
       <c r="B54" t="n">
         <v>108561</v>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -984,6 +1254,11 @@
       <c r="B55" t="n">
         <v>109958</v>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -994,6 +1269,11 @@
       <c r="B56" t="n">
         <v>100333</v>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1004,6 +1284,11 @@
       <c r="B57" t="n">
         <v>77502</v>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1014,6 +1299,11 @@
       <c r="B58" t="n">
         <v>62009</v>
       </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1024,6 +1314,11 @@
       <c r="B59" t="n">
         <v>45142</v>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1034,6 +1329,11 @@
       <c r="B60" t="n">
         <v>62552</v>
       </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1044,6 +1344,11 @@
       <c r="B61" t="n">
         <v>94531</v>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1054,6 +1359,11 @@
       <c r="B62" t="n">
         <v>87850</v>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1064,6 +1374,11 @@
       <c r="B63" t="n">
         <v>156493</v>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1074,6 +1389,11 @@
       <c r="B64" t="n">
         <v>57218</v>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1084,6 +1404,11 @@
       <c r="B65" t="n">
         <v>106213</v>
       </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1094,6 +1419,11 @@
       <c r="B66" t="n">
         <v>58706</v>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1104,6 +1434,11 @@
       <c r="B67" t="n">
         <v>34372</v>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1114,6 +1449,11 @@
       <c r="B68" t="n">
         <v>112384</v>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1124,6 +1464,11 @@
       <c r="B69" t="n">
         <v>58298</v>
       </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1134,6 +1479,11 @@
       <c r="B70" t="n">
         <v>55530</v>
       </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1144,6 +1494,11 @@
       <c r="B71" t="n">
         <v>71432</v>
       </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1154,6 +1509,11 @@
       <c r="B72" t="n">
         <v>81944</v>
       </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1164,6 +1524,11 @@
       <c r="B73" t="n">
         <v>37989</v>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1174,6 +1539,11 @@
       <c r="B74" t="n">
         <v>105354</v>
       </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1184,6 +1554,11 @@
       <c r="B75" t="n">
         <v>56942</v>
       </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1194,6 +1569,11 @@
       <c r="B76" t="n">
         <v>61135</v>
       </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1204,6 +1584,11 @@
       <c r="B77" t="n">
         <v>338586</v>
       </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1214,6 +1599,11 @@
       <c r="B78" t="n">
         <v>62785</v>
       </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1224,6 +1614,11 @@
       <c r="B79" t="n">
         <v>72291</v>
       </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1234,6 +1629,11 @@
       <c r="B80" t="n">
         <v>54598</v>
       </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1244,6 +1644,11 @@
       <c r="B81" t="n">
         <v>57100</v>
       </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1254,6 +1659,11 @@
       <c r="B82" t="n">
         <v>85733</v>
       </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1264,6 +1674,11 @@
       <c r="B83" t="n">
         <v>46944</v>
       </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1274,6 +1689,11 @@
       <c r="B84" t="n">
         <v>48621</v>
       </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1284,6 +1704,11 @@
       <c r="B85" t="n">
         <v>35000</v>
       </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1294,6 +1719,11 @@
       <c r="B86" t="n">
         <v>55520</v>
       </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1304,6 +1734,11 @@
       <c r="B87" t="n">
         <v>75673</v>
       </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1314,6 +1749,11 @@
       <c r="B88" t="n">
         <v>78148</v>
       </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1324,6 +1764,11 @@
       <c r="B89" t="n">
         <v>95423</v>
       </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1334,6 +1779,11 @@
       <c r="B90" t="n">
         <v>38613</v>
       </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1344,6 +1794,11 @@
       <c r="B91" t="n">
         <v>122589</v>
       </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1354,6 +1809,11 @@
       <c r="B92" t="n">
         <v>140892</v>
       </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1364,6 +1824,11 @@
       <c r="B93" t="n">
         <v>112443</v>
       </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1374,6 +1839,11 @@
       <c r="B94" t="n">
         <v>95516</v>
       </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1384,6 +1854,11 @@
       <c r="B95" t="n">
         <v>49736</v>
       </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1394,6 +1869,11 @@
       <c r="B96" t="n">
         <v>49286</v>
       </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1404,6 +1884,11 @@
       <c r="B97" t="n">
         <v>77614</v>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1414,6 +1899,11 @@
       <c r="B98" t="n">
         <v>72565</v>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1424,6 +1914,11 @@
       <c r="B99" t="n">
         <v>75524</v>
       </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1434,6 +1929,11 @@
       <c r="B100" t="n">
         <v>118941</v>
       </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1444,6 +1944,11 @@
       <c r="B101" t="n">
         <v>50952</v>
       </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1454,6 +1959,11 @@
       <c r="B102" t="n">
         <v>91208</v>
       </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1464,6 +1974,11 @@
       <c r="B103" t="n">
         <v>40906</v>
       </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1474,6 +1989,11 @@
       <c r="B104" t="n">
         <v>111696</v>
       </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1484,6 +2004,11 @@
       <c r="B105" t="n">
         <v>48385</v>
       </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1494,6 +2019,11 @@
       <c r="B106" t="n">
         <v>116918</v>
       </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1504,6 +2034,11 @@
       <c r="B107" t="n">
         <v>38173</v>
       </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1514,6 +2049,11 @@
       <c r="B108" t="n">
         <v>115735</v>
       </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1524,6 +2064,11 @@
       <c r="B109" t="n">
         <v>75736</v>
       </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1534,6 +2079,11 @@
       <c r="B110" t="n">
         <v>41984</v>
       </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1544,6 +2094,11 @@
       <c r="B111" t="n">
         <v>66064</v>
       </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1554,6 +2109,11 @@
       <c r="B112" t="n">
         <v>165850</v>
       </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1564,6 +2124,11 @@
       <c r="B113" t="n">
         <v>30648</v>
       </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1574,6 +2139,11 @@
       <c r="B114" t="n">
         <v>672185</v>
       </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1584,6 +2154,11 @@
       <c r="B115" t="n">
         <v>72250</v>
       </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -1594,6 +2169,11 @@
       <c r="B116" t="n">
         <v>47655</v>
       </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -1604,6 +2184,11 @@
       <c r="B117" t="n">
         <v>106947</v>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -1614,6 +2199,11 @@
       <c r="B118" t="n">
         <v>93035</v>
       </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1624,6 +2214,11 @@
       <c r="B119" t="n">
         <v>123664</v>
       </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -1634,6 +2229,11 @@
       <c r="B120" t="n">
         <v>58977</v>
       </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -1644,6 +2244,11 @@
       <c r="B121" t="n">
         <v>108487</v>
       </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -1654,6 +2259,11 @@
       <c r="B122" t="n">
         <v>281440</v>
       </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -1664,6 +2274,11 @@
       <c r="B123" t="n">
         <v>132148</v>
       </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -1674,6 +2289,11 @@
       <c r="B124" t="n">
         <v>48464</v>
       </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -1684,6 +2304,11 @@
       <c r="B125" t="n">
         <v>127972</v>
       </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -1694,6 +2319,11 @@
       <c r="B126" t="n">
         <v>217071</v>
       </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -1704,6 +2334,11 @@
       <c r="B127" t="n">
         <v>191646</v>
       </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -1714,6 +2349,11 @@
       <c r="B128" t="n">
         <v>110471</v>
       </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -1724,6 +2364,11 @@
       <c r="B129" t="n">
         <v>152687</v>
       </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -1734,6 +2379,11 @@
       <c r="B130" t="n">
         <v>43057</v>
       </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -1744,6 +2394,11 @@
       <c r="B131" t="n">
         <v>83761</v>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -1754,6 +2409,11 @@
       <c r="B132" t="n">
         <v>201230</v>
       </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -1764,6 +2424,11 @@
       <c r="B133" t="n">
         <v>68049</v>
       </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -1774,6 +2439,11 @@
       <c r="B134" t="n">
         <v>159662</v>
       </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -1784,6 +2454,11 @@
       <c r="B135" t="n">
         <v>130651</v>
       </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -1794,6 +2469,11 @@
       <c r="B136" t="n">
         <v>779966</v>
       </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -1804,6 +2484,11 @@
       <c r="B137" t="n">
         <v>83558</v>
       </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -1814,6 +2499,11 @@
       <c r="B138" t="n">
         <v>107498</v>
       </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -1824,6 +2514,11 @@
       <c r="B139" t="n">
         <v>33329</v>
       </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -1834,6 +2529,11 @@
       <c r="B140" t="n">
         <v>88891</v>
       </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -1844,6 +2544,11 @@
       <c r="B141" t="n">
         <v>108634</v>
       </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -1854,6 +2559,11 @@
       <c r="B142" t="n">
         <v>44581</v>
       </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -1864,6 +2574,11 @@
       <c r="B143" t="n">
         <v>97462</v>
       </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -1874,6 +2589,11 @@
       <c r="B144" t="n">
         <v>97979</v>
       </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -1884,6 +2604,11 @@
       <c r="B145" t="n">
         <v>59592</v>
       </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -1894,6 +2619,11 @@
       <c r="B146" t="n">
         <v>119882</v>
       </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -1904,6 +2634,11 @@
       <c r="B147" t="n">
         <v>33598</v>
       </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -1914,6 +2649,11 @@
       <c r="B148" t="n">
         <v>30556</v>
       </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -1924,6 +2664,11 @@
       <c r="B149" t="n">
         <v>44438</v>
       </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -1934,6 +2679,11 @@
       <c r="B150" t="n">
         <v>154951</v>
       </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -1944,6 +2694,11 @@
       <c r="B151" t="n">
         <v>72269</v>
       </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -1954,6 +2709,11 @@
       <c r="B152" t="n">
         <v>79265</v>
       </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -1964,6 +2724,11 @@
       <c r="B153" t="n">
         <v>88497</v>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -1974,6 +2739,11 @@
       <c r="B154" t="n">
         <v>71790</v>
       </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -1984,6 +2754,11 @@
       <c r="B155" t="n">
         <v>124283</v>
       </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -1994,6 +2769,11 @@
       <c r="B156" t="n">
         <v>190606</v>
       </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2004,6 +2784,11 @@
       <c r="B157" t="n">
         <v>110742</v>
       </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2014,6 +2799,11 @@
       <c r="B158" t="n">
         <v>86671</v>
       </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2024,6 +2814,11 @@
       <c r="B159" t="n">
         <v>166679</v>
       </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2034,6 +2829,11 @@
       <c r="B160" t="n">
         <v>52101</v>
       </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2044,6 +2844,11 @@
       <c r="B161" t="n">
         <v>41126</v>
       </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2054,6 +2859,11 @@
       <c r="B162" t="n">
         <v>51741</v>
       </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2064,6 +2874,11 @@
       <c r="B163" t="n">
         <v>152190</v>
       </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2074,6 +2889,11 @@
       <c r="B164" t="n">
         <v>81385</v>
       </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2084,6 +2904,11 @@
       <c r="B165" t="n">
         <v>51534</v>
       </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2094,6 +2919,11 @@
       <c r="B166" t="n">
         <v>84804</v>
       </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -2104,6 +2934,11 @@
       <c r="B167" t="n">
         <v>53294</v>
       </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -2114,6 +2949,11 @@
       <c r="B168" t="n">
         <v>39340</v>
       </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -2124,6 +2964,11 @@
       <c r="B169" t="n">
         <v>120144</v>
       </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -2134,6 +2979,11 @@
       <c r="B170" t="n">
         <v>65410</v>
       </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -2144,6 +2994,11 @@
       <c r="B171" t="n">
         <v>252408</v>
       </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -2154,6 +3009,11 @@
       <c r="B172" t="n">
         <v>74210</v>
       </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -2164,6 +3024,11 @@
       <c r="B173" t="n">
         <v>35875</v>
       </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -2174,6 +3039,11 @@
       <c r="B174" t="n">
         <v>38202</v>
       </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -2184,6 +3054,11 @@
       <c r="B175" t="n">
         <v>75370</v>
       </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -2194,6 +3069,11 @@
       <c r="B176" t="n">
         <v>51656</v>
       </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -2204,6 +3084,11 @@
       <c r="B177" t="n">
         <v>118268</v>
       </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -2214,6 +3099,11 @@
       <c r="B178" t="n">
         <v>209296</v>
       </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -2224,6 +3114,11 @@
       <c r="B179" t="n">
         <v>77813</v>
       </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -2234,6 +3129,11 @@
       <c r="B180" t="n">
         <v>1794166</v>
       </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -2244,6 +3144,11 @@
       <c r="B181" t="n">
         <v>89282</v>
       </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -2254,6 +3159,11 @@
       <c r="B182" t="n">
         <v>45015</v>
       </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -2264,6 +3174,11 @@
       <c r="B183" t="n">
         <v>93001</v>
       </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -2274,6 +3189,11 @@
       <c r="B184" t="n">
         <v>65026</v>
       </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -2284,6 +3204,11 @@
       <c r="B185" t="n">
         <v>63196</v>
       </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -2294,6 +3219,11 @@
       <c r="B186" t="n">
         <v>42543</v>
       </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -2304,6 +3234,11 @@
       <c r="B187" t="n">
         <v>134864</v>
       </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -2314,6 +3249,11 @@
       <c r="B188" t="n">
         <v>63788</v>
       </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -2324,6 +3264,11 @@
       <c r="B189" t="n">
         <v>123532</v>
       </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -2334,6 +3279,11 @@
       <c r="B190" t="n">
         <v>54765</v>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -2344,6 +3294,11 @@
       <c r="B191" t="n">
         <v>73923</v>
       </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -2354,6 +3309,11 @@
       <c r="B192" t="n">
         <v>127839</v>
       </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -2364,6 +3324,11 @@
       <c r="B193" t="n">
         <v>21489</v>
       </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -2374,6 +3339,11 @@
       <c r="B194" t="n">
         <v>65373</v>
       </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -2384,6 +3354,11 @@
       <c r="B195" t="n">
         <v>134991</v>
       </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -2394,6 +3369,11 @@
       <c r="B196" t="n">
         <v>119727</v>
       </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -2404,6 +3384,11 @@
       <c r="B197" t="n">
         <v>112863</v>
       </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -2414,6 +3399,11 @@
       <c r="B198" t="n">
         <v>62039</v>
       </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -2424,6 +3414,11 @@
       <c r="B199" t="n">
         <v>111905</v>
       </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -2434,6 +3429,11 @@
       <c r="B200" t="n">
         <v>68996</v>
       </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -2444,6 +3444,11 @@
       <c r="B201" t="n">
         <v>54711</v>
       </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -2454,6 +3459,11 @@
       <c r="B202" t="n">
         <v>81226</v>
       </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -2464,6 +3474,11 @@
       <c r="B203" t="n">
         <v>136441</v>
       </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -2474,6 +3489,11 @@
       <c r="B204" t="n">
         <v>66221</v>
       </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -2484,6 +3504,11 @@
       <c r="B205" t="n">
         <v>73919</v>
       </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -2494,6 +3519,11 @@
       <c r="B206" t="n">
         <v>77979</v>
       </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -2504,6 +3534,11 @@
       <c r="B207" t="n">
         <v>74573</v>
       </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -2514,6 +3549,11 @@
       <c r="B208" t="n">
         <v>170550</v>
       </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -2524,6 +3564,11 @@
       <c r="B209" t="n">
         <v>93818</v>
       </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -2534,6 +3579,11 @@
       <c r="B210" t="n">
         <v>105431</v>
       </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -2544,6 +3594,11 @@
       <c r="B211" t="n">
         <v>61161</v>
       </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -2554,6 +3609,11 @@
       <c r="B212" t="n">
         <v>52720</v>
       </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -2564,6 +3624,11 @@
       <c r="B213" t="n">
         <v>26375</v>
       </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -2574,6 +3639,11 @@
       <c r="B214" t="n">
         <v>45944</v>
       </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -2584,6 +3654,11 @@
       <c r="B215" t="n">
         <v>59779</v>
       </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -2594,6 +3669,11 @@
       <c r="B216" t="n">
         <v>196638</v>
       </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -2604,6 +3684,11 @@
       <c r="B217" t="n">
         <v>46360</v>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -2614,6 +3699,11 @@
       <c r="B218" t="n">
         <v>57651</v>
       </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -2624,6 +3714,11 @@
       <c r="B219" t="n">
         <v>150845</v>
       </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -2634,6 +3729,11 @@
       <c r="B220" t="n">
         <v>53695</v>
       </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -2644,6 +3744,11 @@
       <c r="B221" t="n">
         <v>46792</v>
       </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -2654,6 +3759,11 @@
       <c r="B222" t="n">
         <v>41991</v>
       </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -2664,6 +3774,11 @@
       <c r="B223" t="n">
         <v>37887</v>
       </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -2674,6 +3789,11 @@
       <c r="B224" t="n">
         <v>50819</v>
       </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -2684,6 +3804,11 @@
       <c r="B225" t="n">
         <v>40070</v>
       </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -2694,6 +3819,11 @@
       <c r="B226" t="n">
         <v>19689</v>
       </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -2704,6 +3834,11 @@
       <c r="B227" t="n">
         <v>43618</v>
       </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -2714,6 +3849,11 @@
       <c r="B228" t="n">
         <v>65883</v>
       </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -2724,6 +3864,11 @@
       <c r="B229" t="n">
         <v>35577</v>
       </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -2734,6 +3879,11 @@
       <c r="B230" t="n">
         <v>56408</v>
       </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -2744,6 +3894,11 @@
       <c r="B231" t="n">
         <v>43191</v>
       </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -2754,6 +3909,11 @@
       <c r="B232" t="n">
         <v>296958</v>
       </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -2764,6 +3924,11 @@
       <c r="B233" t="n">
         <v>62573</v>
       </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -2774,6 +3939,11 @@
       <c r="B234" t="n">
         <v>69639</v>
       </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -2784,6 +3954,11 @@
       <c r="B235" t="n">
         <v>79114</v>
       </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -2794,6 +3969,11 @@
       <c r="B236" t="n">
         <v>97661</v>
       </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -2804,6 +3984,11 @@
       <c r="B237" t="n">
         <v>55835</v>
       </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -2814,6 +3999,11 @@
       <c r="B238" t="n">
         <v>120327</v>
       </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -2824,6 +4014,11 @@
       <c r="B239" t="n">
         <v>141892</v>
       </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -2834,6 +4029,11 @@
       <c r="B240" t="n">
         <v>72923</v>
       </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -2844,6 +4044,11 @@
       <c r="B241" t="n">
         <v>82963</v>
       </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -2854,6 +4059,11 @@
       <c r="B242" t="n">
         <v>66083</v>
       </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -2864,6 +4074,11 @@
       <c r="B243" t="n">
         <v>63204</v>
       </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -2874,6 +4089,11 @@
       <c r="B244" t="n">
         <v>35438</v>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -2884,6 +4104,11 @@
       <c r="B245" t="n">
         <v>87568</v>
       </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -2894,6 +4119,11 @@
       <c r="B246" t="n">
         <v>98832</v>
       </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -2904,6 +4134,11 @@
       <c r="B247" t="n">
         <v>128210</v>
       </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -2914,6 +4149,11 @@
       <c r="B248" t="n">
         <v>115220</v>
       </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -2924,6 +4164,11 @@
       <c r="B249" t="n">
         <v>219457</v>
       </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -2934,6 +4179,11 @@
       <c r="B250" t="n">
         <v>41104</v>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -2944,6 +4194,11 @@
       <c r="B251" t="n">
         <v>470805</v>
       </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -2954,6 +4209,11 @@
       <c r="B252" t="n">
         <v>244969</v>
       </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -2964,6 +4224,11 @@
       <c r="B253" t="n">
         <v>89780</v>
       </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -2974,6 +4239,11 @@
       <c r="B254" t="n">
         <v>35286</v>
       </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -2984,6 +4254,11 @@
       <c r="B255" t="n">
         <v>147259</v>
       </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -2994,6 +4269,11 @@
       <c r="B256" t="n">
         <v>166348</v>
       </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -3004,6 +4284,11 @@
       <c r="B257" t="n">
         <v>177536</v>
       </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -3014,6 +4299,11 @@
       <c r="B258" t="n">
         <v>134106</v>
       </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -3024,6 +4314,11 @@
       <c r="B259" t="n">
         <v>115416</v>
       </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -3034,6 +4329,11 @@
       <c r="B260" t="n">
         <v>84330</v>
       </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -3044,6 +4344,11 @@
       <c r="B261" t="n">
         <v>76109</v>
       </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -3054,6 +4359,11 @@
       <c r="B262" t="n">
         <v>99202</v>
       </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -3064,6 +4374,11 @@
       <c r="B263" t="n">
         <v>70486</v>
       </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -3074,6 +4389,11 @@
       <c r="B264" t="n">
         <v>111814</v>
       </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -3084,6 +4404,11 @@
       <c r="B265" t="n">
         <v>107410</v>
       </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -3094,6 +4419,11 @@
       <c r="B266" t="n">
         <v>78166</v>
       </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -3104,6 +4434,11 @@
       <c r="B267" t="n">
         <v>140780</v>
       </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -3114,6 +4449,11 @@
       <c r="B268" t="n">
         <v>59823</v>
       </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -3124,6 +4464,11 @@
       <c r="B269" t="n">
         <v>156579</v>
       </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -3134,6 +4479,11 @@
       <c r="B270" t="n">
         <v>116672</v>
       </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -3144,6 +4494,11 @@
       <c r="B271" t="n">
         <v>152199</v>
       </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -3154,6 +4509,11 @@
       <c r="B272" t="n">
         <v>169756</v>
       </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -3164,6 +4524,11 @@
       <c r="B273" t="n">
         <v>163255</v>
       </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -3174,6 +4539,11 @@
       <c r="B274" t="n">
         <v>106846</v>
       </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -3184,6 +4554,11 @@
       <c r="B275" t="n">
         <v>217530</v>
       </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -3194,6 +4569,11 @@
       <c r="B276" t="n">
         <v>118285</v>
       </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -3204,6 +4584,11 @@
       <c r="B277" t="n">
         <v>177049</v>
       </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -3214,6 +4599,11 @@
       <c r="B278" t="n">
         <v>88038</v>
       </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -3224,6 +4614,11 @@
       <c r="B279" t="n">
         <v>90368</v>
       </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -3234,6 +4629,11 @@
       <c r="B280" t="n">
         <v>290553</v>
       </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -3244,6 +4644,11 @@
       <c r="B281" t="n">
         <v>74559</v>
       </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -3254,6 +4659,11 @@
       <c r="B282" t="n">
         <v>54702</v>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -3264,6 +4674,11 @@
       <c r="B283" t="n">
         <v>136423</v>
       </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -3274,6 +4689,11 @@
       <c r="B284" t="n">
         <v>137128</v>
       </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -3284,6 +4704,11 @@
       <c r="B285" t="n">
         <v>66270</v>
       </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -3294,6 +4719,11 @@
       <c r="B286" t="n">
         <v>197586</v>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -3304,6 +4734,11 @@
       <c r="B287" t="n">
         <v>49108</v>
       </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -3314,6 +4749,11 @@
       <c r="B288" t="n">
         <v>126871</v>
       </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -3324,6 +4764,11 @@
       <c r="B289" t="n">
         <v>170924</v>
       </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -3334,6 +4779,11 @@
       <c r="B290" t="n">
         <v>62844</v>
       </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -3344,6 +4794,11 @@
       <c r="B291" t="n">
         <v>71125</v>
       </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -3354,6 +4809,11 @@
       <c r="B292" t="n">
         <v>84908</v>
       </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -3364,6 +4824,11 @@
       <c r="B293" t="n">
         <v>33340</v>
       </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -3374,6 +4839,11 @@
       <c r="B294" t="n">
         <v>210992</v>
       </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -3384,6 +4854,11 @@
       <c r="B295" t="n">
         <v>79072</v>
       </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -3394,6 +4869,11 @@
       <c r="B296" t="n">
         <v>51525</v>
       </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -3404,6 +4884,11 @@
       <c r="B297" t="n">
         <v>107711</v>
       </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -3414,6 +4899,11 @@
       <c r="B298" t="n">
         <v>38487</v>
       </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -3424,6 +4914,11 @@
       <c r="B299" t="n">
         <v>76346</v>
       </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -3434,6 +4929,11 @@
       <c r="B300" t="n">
         <v>73163</v>
       </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -3444,6 +4944,11 @@
       <c r="B301" t="n">
         <v>88549</v>
       </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -3454,6 +4959,11 @@
       <c r="B302" t="n">
         <v>71250</v>
       </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -3464,6 +4974,11 @@
       <c r="B303" t="n">
         <v>44743</v>
       </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -3474,6 +4989,11 @@
       <c r="B304" t="n">
         <v>193415</v>
       </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -3484,6 +5004,11 @@
       <c r="B305" t="n">
         <v>56562</v>
       </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -3494,6 +5019,11 @@
       <c r="B306" t="n">
         <v>40776</v>
       </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -3504,6 +5034,11 @@
       <c r="B307" t="n">
         <v>64768</v>
       </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -3514,6 +5049,11 @@
       <c r="B308" t="n">
         <v>56986</v>
       </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -3524,6 +5064,11 @@
       <c r="B309" t="n">
         <v>91395</v>
       </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -3534,6 +5079,11 @@
       <c r="B310" t="n">
         <v>56227</v>
       </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -3544,6 +5094,11 @@
       <c r="B311" t="n">
         <v>92644</v>
       </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -3554,6 +5109,11 @@
       <c r="B312" t="n">
         <v>61772</v>
       </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -3564,6 +5124,11 @@
       <c r="B313" t="n">
         <v>40852</v>
       </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -3574,6 +5139,11 @@
       <c r="B314" t="n">
         <v>49439</v>
       </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -3584,6 +5154,11 @@
       <c r="B315" t="n">
         <v>32638</v>
       </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -3594,6 +5169,11 @@
       <c r="B316" t="n">
         <v>43721</v>
       </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -3604,6 +5184,11 @@
       <c r="B317" t="n">
         <v>33993</v>
       </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -3614,6 +5199,11 @@
       <c r="B318" t="n">
         <v>127544</v>
       </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -3624,6 +5214,11 @@
       <c r="B319" t="n">
         <v>103492</v>
       </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -3634,6 +5229,11 @@
       <c r="B320" t="n">
         <v>55833</v>
       </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -3644,6 +5244,11 @@
       <c r="B321" t="n">
         <v>69089</v>
       </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -3654,6 +5259,11 @@
       <c r="B322" t="n">
         <v>26489</v>
       </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -3664,6 +5274,11 @@
       <c r="B323" t="n">
         <v>22444</v>
       </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -3674,6 +5289,11 @@
       <c r="B324" t="n">
         <v>118582</v>
       </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -3684,6 +5304,11 @@
       <c r="B325" t="n">
         <v>171249</v>
       </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -3694,6 +5319,11 @@
       <c r="B326" t="n">
         <v>46824</v>
       </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -3704,6 +5334,11 @@
       <c r="B327" t="n">
         <v>86590</v>
       </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -3714,6 +5349,11 @@
       <c r="B328" t="n">
         <v>145068</v>
       </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -3724,6 +5364,11 @@
       <c r="B329" t="n">
         <v>75732</v>
       </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -3734,6 +5379,11 @@
       <c r="B330" t="n">
         <v>51929</v>
       </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -3744,6 +5394,11 @@
       <c r="B331" t="n">
         <v>71425</v>
       </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -3754,6 +5409,11 @@
       <c r="B332" t="n">
         <v>82911</v>
       </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -3764,6 +5424,11 @@
       <c r="B333" t="n">
         <v>56298</v>
       </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -3774,6 +5439,11 @@
       <c r="B334" t="n">
         <v>86108</v>
       </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -3784,6 +5454,11 @@
       <c r="B335" t="n">
         <v>129904</v>
       </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -3794,6 +5469,11 @@
       <c r="B336" t="n">
         <v>78866</v>
       </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -3804,6 +5484,11 @@
       <c r="B337" t="n">
         <v>76998</v>
       </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -3814,6 +5499,11 @@
       <c r="B338" t="n">
         <v>57911</v>
       </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -3824,6 +5514,11 @@
       <c r="B339" t="n">
         <v>36633</v>
       </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -3834,6 +5529,11 @@
       <c r="B340" t="n">
         <v>75576</v>
       </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -3844,6 +5544,11 @@
       <c r="B341" t="n">
         <v>59821</v>
       </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -3854,6 +5559,11 @@
       <c r="B342" t="n">
         <v>161357</v>
       </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -3864,6 +5574,11 @@
       <c r="B343" t="n">
         <v>55265</v>
       </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -3874,6 +5589,11 @@
       <c r="B344" t="n">
         <v>135477</v>
       </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -3884,6 +5604,11 @@
       <c r="B345" t="n">
         <v>62763</v>
       </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -3894,6 +5619,11 @@
       <c r="B346" t="n">
         <v>406590</v>
       </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -3904,6 +5634,11 @@
       <c r="B347" t="n">
         <v>60188</v>
       </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -3914,6 +5649,11 @@
       <c r="B348" t="n">
         <v>58959</v>
       </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -3924,6 +5664,11 @@
       <c r="B349" t="n">
         <v>91745</v>
       </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -3934,6 +5679,11 @@
       <c r="B350" t="n">
         <v>59149</v>
       </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -3944,6 +5694,11 @@
       <c r="B351" t="n">
         <v>61492</v>
       </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -3954,6 +5709,11 @@
       <c r="B352" t="n">
         <v>83599</v>
       </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -3964,6 +5724,11 @@
       <c r="B353" t="n">
         <v>70096</v>
       </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -3974,6 +5739,11 @@
       <c r="B354" t="n">
         <v>57431</v>
       </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -3984,6 +5754,11 @@
       <c r="B355" t="n">
         <v>78037</v>
       </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -3994,6 +5769,11 @@
       <c r="B356" t="n">
         <v>69161</v>
       </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -4004,6 +5784,11 @@
       <c r="B357" t="n">
         <v>99106</v>
       </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -4014,6 +5799,11 @@
       <c r="B358" t="n">
         <v>72539</v>
       </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -4024,6 +5814,11 @@
       <c r="B359" t="n">
         <v>62854</v>
       </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -4034,6 +5829,11 @@
       <c r="B360" t="n">
         <v>532048</v>
       </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -4044,6 +5844,11 @@
       <c r="B361" t="n">
         <v>47304</v>
       </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -4054,6 +5859,11 @@
       <c r="B362" t="n">
         <v>47970</v>
       </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -4064,6 +5874,11 @@
       <c r="B363" t="n">
         <v>56482</v>
       </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -4074,6 +5889,11 @@
       <c r="B364" t="n">
         <v>82310</v>
       </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -4084,6 +5904,11 @@
       <c r="B365" t="n">
         <v>59844</v>
       </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -4094,6 +5919,11 @@
       <c r="B366" t="n">
         <v>81289</v>
       </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -4104,6 +5934,11 @@
       <c r="B367" t="n">
         <v>46692</v>
       </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -4114,6 +5949,11 @@
       <c r="B368" t="n">
         <v>79300</v>
       </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -4124,6 +5964,11 @@
       <c r="B369" t="n">
         <v>66505</v>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -4134,6 +5979,11 @@
       <c r="B370" t="n">
         <v>65373</v>
       </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -4144,6 +5994,11 @@
       <c r="B371" t="n">
         <v>81584</v>
       </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -4154,6 +6009,11 @@
       <c r="B372" t="n">
         <v>39202</v>
       </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -4164,6 +6024,11 @@
       <c r="B373" t="n">
         <v>55777</v>
       </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -4174,6 +6039,11 @@
       <c r="B374" t="n">
         <v>120132</v>
       </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -4184,6 +6054,11 @@
       <c r="B375" t="n">
         <v>77258</v>
       </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -4194,6 +6069,11 @@
       <c r="B376" t="n">
         <v>46394</v>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -4204,6 +6084,11 @@
       <c r="B377" t="n">
         <v>52707</v>
       </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -4214,6 +6099,11 @@
       <c r="B378" t="n">
         <v>36486</v>
       </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -4224,6 +6114,11 @@
       <c r="B379" t="n">
         <v>106235</v>
       </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -4234,6 +6129,11 @@
       <c r="B380" t="n">
         <v>398255</v>
       </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -4243,6 +6143,11 @@
       </c>
       <c r="B381" t="n">
         <v>40948</v>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>2021-08-07</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>